<commit_message>
Inhalt des Commits: aktualisierte Variante des Zeiplans
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktoria Horn\Documents\Studium\3. Semester\03Modul_Medienproduktion\3D-Modellierung und Animation\Projektphase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktoria Horn\Documents\Studium\3. Semester\03Modul_Medienproduktion\3D-Modellierung und Animation\Projektphase\Nachts-im-Kinderzimmer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -567,6 +567,9 @@
     <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -575,9 +578,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -587,141 +587,23 @@
     <cellStyle name="Überschrift 1" xfId="4" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="15">
     <dxf>
       <font>
-        <color theme="4" tint="-0.499984740745262"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -746,23 +628,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -870,6 +735,21 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4"/>
@@ -924,11 +804,11 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Project To Do List" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Project To Do List" pivot="0" count="5">
-      <tableStyleElement type="wholeTable" dxfId="22"/>
-      <tableStyleElement type="headerRow" dxfId="21"/>
-      <tableStyleElement type="totalRow" dxfId="20"/>
-      <tableStyleElement type="firstRowStripe" dxfId="19"/>
-      <tableStyleElement type="secondRowStripe" dxfId="18"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -942,98 +822,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>352426</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Tipp zum Filtern oder Sortieren" descr="Click the drop down arrows in the table header row to filter or sort your project information" title="Tip"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7915275" y="2076449"/>
-          <a:ext cx="1647826" cy="1181101"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:lumMod val="20000"/>
-              <a:lumOff val="80000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="1">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>TIPP: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Klicken Sie auf die Dropdownpfeile in der Tabellenkopfzeile, um die Projektinformationen zu filtern oder zu sortieren. </a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData fPrintsWithSheet="0"/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblAufgabenliste" displayName="tblAufgabenliste" ref="B9:H52">
   <autoFilter ref="B9:H52"/>
@@ -1041,15 +829,15 @@
     <sortCondition ref="C9:C47"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="17"/>
-    <tableColumn id="7" name="Fällig am" totalsRowDxfId="16"/>
-    <tableColumn id="4" name="Person" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="1" name="% erledigt" totalsRowDxfId="13"/>
-    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="12">
+    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="8"/>
+    <tableColumn id="7" name="Fällig am" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Person" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="1" name="% erledigt" totalsRowDxfId="4"/>
+    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="3">
       <calculatedColumnFormula>tblAufgabenliste[[#This Row],[% erledigt]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="11"/>
-    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="9" totalsRowDxfId="10"/>
+    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="2"/>
+    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Project To Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1293,8 +1081,8 @@
   </sheetPr>
   <dimension ref="B1:I52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46:E48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1349,8 +1137,7 @@
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
       <c r="E6" s="28">
-        <f ca="1">TODAY()+27</f>
-        <v>42353</v>
+        <v>42351</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="27" t="s">
@@ -1358,10 +1145,10 @@
       </c>
     </row>
     <row r="8" spans="2:9" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="42"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1639,7 +1426,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="13"/>
-      <c r="H21" s="44"/>
+      <c r="H21" s="41"/>
     </row>
     <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
@@ -1917,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="13"/>
-      <c r="H35" s="44"/>
+      <c r="H35" s="41"/>
     </row>
     <row r="36" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="13" t="s">
@@ -1937,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="13"/>
-      <c r="H36" s="44"/>
+      <c r="H36" s="41"/>
     </row>
     <row r="37" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="37" t="s">
@@ -2077,7 +1864,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="13"/>
-      <c r="H43" s="44"/>
+      <c r="H43" s="41"/>
     </row>
     <row r="44" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="13" t="s">
@@ -2097,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="13"/>
-      <c r="H44" s="44"/>
+      <c r="H44" s="41"/>
     </row>
     <row r="45" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="37" t="s">
@@ -2157,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="13"/>
-      <c r="H47" s="44"/>
+      <c r="H47" s="41"/>
     </row>
     <row r="48" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="13" t="s">
@@ -2177,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="13"/>
-      <c r="H48" s="44"/>
+      <c r="H48" s="41"/>
     </row>
     <row r="49" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="13" t="s">
@@ -2237,7 +2024,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="13"/>
-      <c r="H51" s="44"/>
+      <c r="H51" s="41"/>
     </row>
     <row r="52" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="37" t="s">
@@ -2264,7 +2051,7 @@
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:H52">
-    <cfRule type="expression" dxfId="2" priority="13">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>($C10&gt;=valHStart)*($C10&lt;=valHEnde)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2292,9 +2079,8 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -2373,12 +2159,12 @@
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
     </row>
     <row r="5" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">

</xml_diff>

<commit_message>
kleine Änderung am Zeitplan(vh)
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -587,22 +587,7 @@
     <cellStyle name="Überschrift 1" xfId="4" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
@@ -819,11 +804,11 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Project To Do List" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Project To Do List" pivot="0" count="5">
-      <tableStyleElement type="wholeTable" dxfId="15"/>
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="totalRow" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -936,15 +921,15 @@
     <sortCondition ref="C9:C47"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="9"/>
-    <tableColumn id="7" name="Fällig am" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="Person" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="1" name="% erledigt" totalsRowDxfId="5"/>
-    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="4">
+    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="8"/>
+    <tableColumn id="7" name="Fällig am" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Person" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="1" name="% erledigt" totalsRowDxfId="4"/>
+    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="3">
       <calculatedColumnFormula>tblAufgabenliste[[#This Row],[% erledigt]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="2"/>
+    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Project To Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1188,8 +1173,8 @@
   </sheetPr>
   <dimension ref="B1:I52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1244,8 +1229,7 @@
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
       <c r="E6" s="28">
-        <f ca="1">TODAY()+27</f>
-        <v>42353</v>
+        <v>42351</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="27" t="s">
@@ -2171,7 +2155,7 @@
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:H52">
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>($C10&gt;=valHStart)*($C10&lt;=valHEnde)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Inhalt des Commits: Aktualisierung des Zeitplans (vh)
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="100">
   <si>
     <t>Start:</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Textur -  Himmel</t>
   </si>
   <si>
-    <t>Textur -  Boden</t>
-  </si>
-  <si>
     <t>Holztexturen -  (Bett, Schrank, Nachttisch)</t>
   </si>
   <si>
@@ -244,9 +241,6 @@
     <t>(M) - Bett + schlafenden Jungen</t>
   </si>
   <si>
-    <t>Textur - Tapete</t>
-  </si>
-  <si>
     <t>Auto ins Git committen</t>
   </si>
   <si>
@@ -265,9 +259,6 @@
     <t xml:space="preserve">Jana </t>
   </si>
   <si>
-    <t>(R) - Rendern des Films</t>
-  </si>
-  <si>
     <t>(S) - Schrank, Mobile, Fenster-Szene fertig stellen</t>
   </si>
   <si>
@@ -284,6 +275,60 @@
   </si>
   <si>
     <t>(A) - Animation der Shots 10 - 14</t>
+  </si>
+  <si>
+    <t>(R) - Rendern des Films + Tonspur + Abspann</t>
+  </si>
+  <si>
+    <t>tatsächliche Fertigstellung</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Textur -  Boden (externe Quelle)</t>
+  </si>
+  <si>
+    <t>Textur - Tapete (externe  Quelle)</t>
+  </si>
+  <si>
+    <t>0,5 h</t>
+  </si>
+  <si>
+    <t>1,5 h</t>
+  </si>
+  <si>
+    <t>3,5h</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>2,5 h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4h </t>
+  </si>
+  <si>
+    <t>4 h</t>
+  </si>
+  <si>
+    <t>2 h</t>
+  </si>
+  <si>
+    <t>5 h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 h </t>
+  </si>
+  <si>
+    <t>1 d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,5 h </t>
   </si>
 </sst>
 </file>
@@ -587,7 +632,108 @@
     <cellStyle name="Überschrift 1" xfId="4" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -735,21 +881,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4"/>
@@ -804,11 +935,11 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Project To Do List" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Project To Do List" pivot="0" count="5">
-      <tableStyleElement type="wholeTable" dxfId="14"/>
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="totalRow" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="secondRowStripe" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="19"/>
+      <tableStyleElement type="headerRow" dxfId="18"/>
+      <tableStyleElement type="totalRow" dxfId="17"/>
+      <tableStyleElement type="firstRowStripe" dxfId="16"/>
+      <tableStyleElement type="secondRowStripe" dxfId="15"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -823,21 +954,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblAufgabenliste" displayName="tblAufgabenliste" ref="B9:H52">
-  <autoFilter ref="B9:H52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblAufgabenliste" displayName="tblAufgabenliste" ref="B9:I52">
+  <autoFilter ref="B9:I52"/>
   <sortState ref="B10:H47">
     <sortCondition ref="C9:C47"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="8"/>
-    <tableColumn id="7" name="Fällig am" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="Person" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="1" name="% erledigt" totalsRowDxfId="4"/>
-    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="3">
+  <tableColumns count="8">
+    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="14"/>
+    <tableColumn id="7" name="Fällig am" totalsRowDxfId="13"/>
+    <tableColumn id="4" name="Person" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="1" name="% erledigt" totalsRowDxfId="10"/>
+    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="9">
       <calculatedColumnFormula>tblAufgabenliste[[#This Row],[% erledigt]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="2"/>
-    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="8"/>
+    <tableColumn id="9" name="tatsächliche Fertigstellung" dataDxfId="3" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="7" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Project To Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1079,10 +1211,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I52"/>
+  <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1098,12 +1230,12 @@
     <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1114,12 +1246,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="2:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B3" s="26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
@@ -1130,7 +1262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="29" t="s">
         <v>26</v>
       </c>
@@ -1144,7 +1276,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:9" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="42" t="s">
         <v>28</v>
       </c>
@@ -1154,7 +1286,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>41</v>
       </c>
@@ -1171,16 +1303,19 @@
         <v>5</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>43</v>
       </c>
@@ -1198,11 +1333,14 @@
         <v>1</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="H10" s="15">
+        <v>42324</v>
+      </c>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>34</v>
       </c>
@@ -1216,15 +1354,17 @@
         <v>0</v>
       </c>
       <c r="F11" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="H11" s="15">
+        <v>42324</v>
+      </c>
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
         <v>44</v>
       </c>
@@ -1232,21 +1372,23 @@
         <v>42326</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E12" s="16">
         <v>0</v>
       </c>
       <c r="F12" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="H12" s="15">
+        <v>42328</v>
+      </c>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>46</v>
       </c>
@@ -1264,11 +1406,12 @@
         <v>0</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>35</v>
       </c>
@@ -1279,18 +1422,20 @@
         <v>40</v>
       </c>
       <c r="E14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H14" s="15">
+        <v>42328</v>
+      </c>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>36</v>
       </c>
@@ -1308,13 +1453,16 @@
         <v>0.5</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="H15" s="15">
+        <v>42329</v>
+      </c>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="15">
         <v>42329</v>
@@ -1330,13 +1478,16 @@
         <v>1</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H16" s="15">
+        <v>42327</v>
+      </c>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="15">
         <v>42329</v>
@@ -1344,19 +1495,24 @@
       <c r="D17" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="16"/>
+      <c r="E17" s="16">
+        <v>1</v>
+      </c>
       <c r="F17" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H17" s="13"/>
-    </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H17" s="15">
+        <v>42328</v>
+      </c>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="15">
         <v>42329</v>
@@ -1372,11 +1528,14 @@
         <v>1</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H18" s="15">
+        <v>42327</v>
+      </c>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>50</v>
       </c>
@@ -1386,17 +1545,22 @@
       <c r="D19" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="16"/>
+      <c r="E19" s="16">
+        <v>0</v>
+      </c>
       <c r="F19" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G19" s="13"/>
+      <c r="G19" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="C20" s="15">
         <v>42330</v>
@@ -1404,17 +1568,22 @@
       <c r="D20" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="16">
+        <v>0</v>
+      </c>
       <c r="F20" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="G20" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="C21" s="15">
         <v>42330</v>
@@ -1422,17 +1591,22 @@
       <c r="D21" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="16">
+        <v>0</v>
+      </c>
       <c r="F21" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="41"/>
-    </row>
-    <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" s="13"/>
+      <c r="I21" s="41"/>
+    </row>
+    <row r="22" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="15">
         <v>42330</v>
@@ -1440,15 +1614,20 @@
       <c r="D22" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="16">
+        <v>0</v>
+      </c>
       <c r="F22" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="13" t="s">
+        <v>88</v>
+      </c>
       <c r="H22" s="13"/>
-    </row>
-    <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="37" t="s">
         <v>30</v>
       </c>
@@ -1459,18 +1638,21 @@
         <v>38</v>
       </c>
       <c r="E23" s="40">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="F23" s="40">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0.3</v>
-      </c>
-      <c r="G23" s="37"/>
+        <v>0.8</v>
+      </c>
+      <c r="G23" s="37" t="s">
+        <v>67</v>
+      </c>
       <c r="H23" s="37"/>
-    </row>
-    <row r="24" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="37"/>
+    </row>
+    <row r="24" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C24" s="15">
         <v>42332</v>
@@ -1481,16 +1663,16 @@
       <c r="E24" s="16">
         <v>0</v>
       </c>
-      <c r="F24" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="13"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="H24" s="13"/>
-    </row>
-    <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" s="15">
         <v>42332</v>
@@ -1505,12 +1687,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G25" s="13"/>
+      <c r="G25" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C26" s="15">
         <v>42332</v>
@@ -1525,10 +1710,13 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G26" s="13"/>
+      <c r="G26" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="H26" s="13"/>
-    </row>
-    <row r="27" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="13" t="s">
         <v>47</v>
       </c>
@@ -1536,7 +1724,7 @@
         <v>42333</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E27" s="16">
         <v>0</v>
@@ -1545,10 +1733,13 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G27" s="13"/>
+      <c r="G27" s="13" t="s">
+        <v>90</v>
+      </c>
       <c r="H27" s="13"/>
-    </row>
-    <row r="28" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="13" t="s">
         <v>48</v>
       </c>
@@ -1556,7 +1747,7 @@
         <v>42333</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E28" s="16">
         <v>0</v>
@@ -1565,12 +1756,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G28" s="13"/>
+      <c r="G28" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="H28" s="13"/>
-    </row>
-    <row r="29" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="15">
         <v>42333</v>
@@ -1585,10 +1779,13 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G29" s="13"/>
+      <c r="G29" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="H29" s="13"/>
-    </row>
-    <row r="30" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="13" t="s">
         <v>49</v>
       </c>
@@ -1605,12 +1802,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G30" s="13"/>
+      <c r="G30" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="H30" s="13"/>
-    </row>
-    <row r="31" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="15">
         <v>42334</v>
@@ -1625,12 +1825,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G31" s="13"/>
+      <c r="G31" s="13" t="s">
+        <v>92</v>
+      </c>
       <c r="H31" s="13"/>
-    </row>
-    <row r="32" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="15">
         <v>42334</v>
@@ -1645,12 +1848,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G32" s="13"/>
+      <c r="G32" s="13" t="s">
+        <v>92</v>
+      </c>
       <c r="H32" s="13"/>
-    </row>
-    <row r="33" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" s="15">
         <v>42334</v>
@@ -1665,10 +1871,13 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G33" s="13"/>
+      <c r="G33" s="13" t="s">
+        <v>92</v>
+      </c>
       <c r="H33" s="13"/>
-    </row>
-    <row r="34" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="13" t="s">
         <v>45</v>
       </c>
@@ -1685,12 +1894,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G34" s="13"/>
+      <c r="G34" s="13" t="s">
+        <v>92</v>
+      </c>
       <c r="H34" s="13"/>
-    </row>
-    <row r="35" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C35" s="15">
         <v>42336</v>
@@ -1705,12 +1917,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="41"/>
-    </row>
-    <row r="36" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="13"/>
+      <c r="I35" s="41"/>
+    </row>
+    <row r="36" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C36" s="15">
         <v>42336</v>
@@ -1725,10 +1940,13 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G36" s="13"/>
-      <c r="H36" s="41"/>
-    </row>
-    <row r="37" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="41"/>
+    </row>
+    <row r="37" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="37" t="s">
         <v>31</v>
       </c>
@@ -1745,12 +1963,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G37" s="37"/>
+      <c r="G37" s="37" t="s">
+        <v>87</v>
+      </c>
       <c r="H37" s="37"/>
-    </row>
-    <row r="38" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="37"/>
+    </row>
+    <row r="38" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="15">
         <v>42339</v>
@@ -1765,12 +1986,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G38" s="13"/>
+      <c r="G38" s="13" t="s">
+        <v>94</v>
+      </c>
       <c r="H38" s="13"/>
-    </row>
-    <row r="39" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" s="15">
         <v>42340</v>
@@ -1785,12 +2009,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G39" s="13"/>
+      <c r="G39" s="13" t="s">
+        <v>95</v>
+      </c>
       <c r="H39" s="13"/>
-    </row>
-    <row r="40" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" s="15">
         <v>42340</v>
@@ -1805,12 +2032,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G40" s="13"/>
+      <c r="G40" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="H40" s="13"/>
-    </row>
-    <row r="41" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" s="15">
         <v>42341</v>
@@ -1825,12 +2055,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G41" s="13"/>
+      <c r="G41" s="13" t="s">
+        <v>95</v>
+      </c>
       <c r="H41" s="13"/>
-    </row>
-    <row r="42" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C42" s="15">
         <v>42343</v>
@@ -1845,12 +2078,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G42" s="13"/>
+      <c r="G42" s="13" t="s">
+        <v>96</v>
+      </c>
       <c r="H42" s="13"/>
-    </row>
-    <row r="43" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I42" s="13"/>
+    </row>
+    <row r="43" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C43" s="15">
         <v>42343</v>
@@ -1865,12 +2101,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G43" s="13"/>
-      <c r="H43" s="41"/>
-    </row>
-    <row r="44" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G43" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H43" s="13"/>
+      <c r="I43" s="41"/>
+    </row>
+    <row r="44" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C44" s="15">
         <v>42343</v>
@@ -1885,10 +2124,13 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G44" s="13"/>
-      <c r="H44" s="41"/>
-    </row>
-    <row r="45" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G44" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H44" s="13"/>
+      <c r="I44" s="41"/>
+    </row>
+    <row r="45" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="37" t="s">
         <v>32</v>
       </c>
@@ -1905,12 +2147,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G45" s="37"/>
+      <c r="G45" s="37" t="s">
+        <v>87</v>
+      </c>
       <c r="H45" s="37"/>
-    </row>
-    <row r="46" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="37"/>
+    </row>
+    <row r="46" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="15">
         <v>42345</v>
@@ -1925,12 +2170,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G46" s="13"/>
+      <c r="G46" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="H46" s="13"/>
-    </row>
-    <row r="47" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="15">
         <v>42347</v>
@@ -1945,12 +2193,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G47" s="13"/>
-      <c r="H47" s="41"/>
-    </row>
-    <row r="48" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G47" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H47" s="13"/>
+      <c r="I47" s="41"/>
+    </row>
+    <row r="48" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" s="15">
         <v>42348</v>
@@ -1965,12 +2216,15 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G48" s="13"/>
-      <c r="H48" s="41"/>
-    </row>
-    <row r="49" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G48" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H48" s="13"/>
+      <c r="I48" s="41"/>
+    </row>
+    <row r="49" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49" s="15">
         <v>42349</v>
@@ -1985,15 +2239,18 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G49" s="13"/>
+      <c r="G49" s="13" t="s">
+        <v>98</v>
+      </c>
       <c r="H49" s="13"/>
-    </row>
-    <row r="50" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="13"/>
+    </row>
+    <row r="50" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="13" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C50" s="15">
-        <v>42349</v>
+        <v>42350</v>
       </c>
       <c r="D50" s="36" t="s">
         <v>37</v>
@@ -2001,16 +2258,16 @@
       <c r="E50" s="16">
         <v>0</v>
       </c>
-      <c r="F50" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="13"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="H50" s="13"/>
-    </row>
-    <row r="51" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C51" s="15">
         <v>42350</v>
@@ -2025,10 +2282,13 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G51" s="13"/>
-      <c r="H51" s="41"/>
-    </row>
-    <row r="52" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H51" s="13"/>
+      <c r="I51" s="41"/>
+    </row>
+    <row r="52" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="37" t="s">
         <v>33</v>
       </c>
@@ -2045,15 +2305,18 @@
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
       </c>
-      <c r="G52" s="37"/>
+      <c r="G52" s="37" t="s">
+        <v>99</v>
+      </c>
       <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B8:C8"/>
   </mergeCells>
-  <conditionalFormatting sqref="B10:H52">
-    <cfRule type="expression" dxfId="9" priority="13">
+  <conditionalFormatting sqref="B10:I52">
+    <cfRule type="expression" dxfId="5" priority="13">
       <formula>($C10&gt;=valHStart)*($C10&lt;=valHEnde)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Inhalt des Commits: Aktualisierung des Zeitplans
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="101">
   <si>
     <t>Start:</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t xml:space="preserve">0,5 h </t>
+  </si>
+  <si>
+    <t>(S) Kamerafahrt-Szene: Bett +Junge</t>
   </si>
 </sst>
 </file>
@@ -632,37 +635,7 @@
     <cellStyle name="Überschrift 1" xfId="4" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color theme="4" tint="-0.499984740745262"/>
@@ -694,13 +667,6 @@
         <name val="Tahoma"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -718,21 +684,13 @@
         <name val="Tahoma"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -935,11 +893,11 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Project To Do List" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Project To Do List" pivot="0" count="5">
-      <tableStyleElement type="wholeTable" dxfId="19"/>
-      <tableStyleElement type="headerRow" dxfId="18"/>
-      <tableStyleElement type="totalRow" dxfId="17"/>
-      <tableStyleElement type="firstRowStripe" dxfId="16"/>
-      <tableStyleElement type="secondRowStripe" dxfId="15"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="secondRowStripe" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -954,22 +912,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblAufgabenliste" displayName="tblAufgabenliste" ref="B9:I52">
-  <autoFilter ref="B9:I52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblAufgabenliste" displayName="tblAufgabenliste" ref="B9:I53">
+  <autoFilter ref="B9:I53"/>
   <sortState ref="B10:H47">
     <sortCondition ref="C9:C47"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="14"/>
-    <tableColumn id="7" name="Fällig am" totalsRowDxfId="13"/>
-    <tableColumn id="4" name="Person" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="1" name="% erledigt" totalsRowDxfId="10"/>
-    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="9">
+    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="11"/>
+    <tableColumn id="7" name="Fällig am" totalsRowDxfId="10"/>
+    <tableColumn id="4" name="Person" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="1" name="% erledigt" totalsRowDxfId="7"/>
+    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="6">
       <calculatedColumnFormula>tblAufgabenliste[[#This Row],[% erledigt]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="8"/>
-    <tableColumn id="9" name="tatsächliche Fertigstellung" dataDxfId="3" totalsRowDxfId="4"/>
-    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="5"/>
+    <tableColumn id="9" name="tatsächliche Fertigstellung" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="2" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Project To Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1211,10 +1169,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J52"/>
+  <dimension ref="B1:J53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1399,11 +1357,11 @@
         <v>39</v>
       </c>
       <c r="E13" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>67</v>
@@ -1566,7 +1524,7 @@
         <v>42330</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="16">
         <v>0</v>
@@ -1638,16 +1596,18 @@
         <v>38</v>
       </c>
       <c r="E23" s="40">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F23" s="40">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G23" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="H23" s="37"/>
+      <c r="H23" s="38">
+        <v>42329</v>
+      </c>
       <c r="I23" s="37"/>
     </row>
     <row r="24" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1695,13 +1655,13 @@
     </row>
     <row r="26" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="C26" s="15">
         <v>42332</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E26" s="16">
         <v>0</v>
@@ -1711,20 +1671,20 @@
         <v>0</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
+        <v>89</v>
+      </c>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
     </row>
     <row r="27" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="13" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="C27" s="15">
-        <v>42333</v>
+        <v>42332</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="E27" s="16">
         <v>0</v>
@@ -1734,20 +1694,20 @@
         <v>0</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="15">
         <v>42333</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="E28" s="16">
         <v>0</v>
@@ -1757,20 +1717,20 @@
         <v>0</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
     <row r="29" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="13" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C29" s="15">
         <v>42333</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E29" s="16">
         <v>0</v>
@@ -1787,13 +1747,13 @@
     </row>
     <row r="30" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="13" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C30" s="15">
         <v>42333</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E30" s="16">
         <v>0</v>
@@ -1803,20 +1763,20 @@
         <v>0</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
     <row r="31" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C31" s="15">
-        <v>42334</v>
+        <v>42333</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E31" s="16">
         <v>0</v>
@@ -1826,20 +1786,20 @@
         <v>0</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="15">
         <v>42334</v>
       </c>
       <c r="D32" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32" s="16">
         <v>0</v>
@@ -1856,13 +1816,13 @@
     </row>
     <row r="33" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="15">
         <v>42334</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E33" s="16">
         <v>0</v>
@@ -1879,13 +1839,13 @@
     </row>
     <row r="34" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="13" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C34" s="15">
-        <v>42335</v>
+        <v>42334</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E34" s="16">
         <v>0</v>
@@ -1902,13 +1862,13 @@
     </row>
     <row r="35" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="13" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="C35" s="15">
-        <v>42336</v>
+        <v>42335</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E35" s="16">
         <v>0</v>
@@ -1918,20 +1878,20 @@
         <v>0</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H35" s="13"/>
-      <c r="I35" s="41"/>
+      <c r="I35" s="13"/>
     </row>
     <row r="36" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="15">
         <v>42336</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E36" s="16">
         <v>0</v>
@@ -1941,66 +1901,66 @@
         <v>0</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="41"/>
     </row>
     <row r="37" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="15">
+        <v>42336</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="16">
+        <v>0</v>
+      </c>
+      <c r="F37" s="16">
+        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H37" s="13"/>
+      <c r="I37" s="41"/>
+    </row>
+    <row r="38" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C38" s="38">
         <v>42337</v>
       </c>
-      <c r="D37" s="39" t="s">
+      <c r="D38" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="40">
-        <v>0</v>
-      </c>
-      <c r="F37" s="40">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="37" t="s">
+      <c r="E38" s="40">
+        <v>0</v>
+      </c>
+      <c r="F38" s="40">
+        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-    </row>
-    <row r="38" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="15">
-        <v>42339</v>
-      </c>
-      <c r="D38" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="16">
-        <v>0</v>
-      </c>
-      <c r="F38" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
     </row>
     <row r="39" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="15">
-        <v>42340</v>
+        <v>42339</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E39" s="16">
         <v>0</v>
@@ -2010,20 +1970,20 @@
         <v>0</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
     </row>
     <row r="40" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="15">
         <v>42340</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E40" s="16">
         <v>0</v>
@@ -2033,20 +1993,20 @@
         <v>0</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
     </row>
     <row r="41" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C41" s="15">
-        <v>42341</v>
+        <v>42340</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E41" s="16">
         <v>0</v>
@@ -2056,20 +2016,20 @@
         <v>0</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
     </row>
     <row r="42" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="13" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="C42" s="15">
-        <v>42343</v>
+        <v>42341</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E42" s="16">
         <v>0</v>
@@ -2079,20 +2039,20 @@
         <v>0</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
     <row r="43" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" s="15">
         <v>42343</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E43" s="16">
         <v>0</v>
@@ -2105,17 +2065,17 @@
         <v>96</v>
       </c>
       <c r="H43" s="13"/>
-      <c r="I43" s="41"/>
+      <c r="I43" s="13"/>
     </row>
     <row r="44" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C44" s="15">
         <v>42343</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E44" s="16">
         <v>0</v>
@@ -2131,57 +2091,57 @@
       <c r="I44" s="41"/>
     </row>
     <row r="45" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="15">
+        <v>42343</v>
+      </c>
+      <c r="D45" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="16">
+        <v>0</v>
+      </c>
+      <c r="F45" s="16">
+        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45" s="13"/>
+      <c r="I45" s="41"/>
+    </row>
+    <row r="46" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="38">
+      <c r="C46" s="38">
         <v>42344</v>
       </c>
-      <c r="D45" s="39" t="s">
+      <c r="D46" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="40">
-        <v>0</v>
-      </c>
-      <c r="F45" s="40">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
-      </c>
-      <c r="G45" s="37" t="s">
+      <c r="E46" s="40">
+        <v>0</v>
+      </c>
+      <c r="F46" s="40">
+        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
-    </row>
-    <row r="46" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="15">
-        <v>42345</v>
-      </c>
-      <c r="D46" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="16">
-        <v>0</v>
-      </c>
-      <c r="F46" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
     </row>
     <row r="47" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47" s="15">
-        <v>42347</v>
+        <v>42345</v>
       </c>
       <c r="D47" s="36" t="s">
         <v>37</v>
@@ -2194,17 +2154,17 @@
         <v>0</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H47" s="13"/>
-      <c r="I47" s="41"/>
+      <c r="I47" s="13"/>
     </row>
     <row r="48" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="13" t="s">
         <v>57</v>
       </c>
       <c r="C48" s="15">
-        <v>42348</v>
+        <v>42347</v>
       </c>
       <c r="D48" s="36" t="s">
         <v>37</v>
@@ -2227,7 +2187,7 @@
         <v>57</v>
       </c>
       <c r="C49" s="15">
-        <v>42349</v>
+        <v>42348</v>
       </c>
       <c r="D49" s="36" t="s">
         <v>37</v>
@@ -2243,14 +2203,14 @@
         <v>98</v>
       </c>
       <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
+      <c r="I49" s="41"/>
     </row>
     <row r="50" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="13" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="C50" s="15">
-        <v>42350</v>
+        <v>42349</v>
       </c>
       <c r="D50" s="36" t="s">
         <v>37</v>
@@ -2258,16 +2218,19 @@
       <c r="E50" s="16">
         <v>0</v>
       </c>
-      <c r="F50" s="16"/>
+      <c r="F50" s="16">
+        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
+        <v>0</v>
+      </c>
       <c r="G50" s="13" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="13" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C51" s="15">
         <v>42350</v>
@@ -2278,50 +2241,70 @@
       <c r="E51" s="16">
         <v>0</v>
       </c>
-      <c r="F51" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
-      </c>
+      <c r="F51" s="16"/>
       <c r="G51" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+    </row>
+    <row r="52" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" s="15">
+        <v>42350</v>
+      </c>
+      <c r="D52" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E52" s="16">
+        <v>0</v>
+      </c>
+      <c r="F52" s="16">
+        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H51" s="13"/>
-      <c r="I51" s="41"/>
-    </row>
-    <row r="52" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="37" t="s">
+      <c r="H52" s="13"/>
+      <c r="I52" s="41"/>
+    </row>
+    <row r="53" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="38">
+      <c r="C53" s="38">
         <v>42351</v>
       </c>
-      <c r="D52" s="39" t="s">
+      <c r="D53" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="E52" s="40">
-        <v>0</v>
-      </c>
-      <c r="F52" s="40">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
-      </c>
-      <c r="G52" s="37" t="s">
+      <c r="E53" s="40">
+        <v>0</v>
+      </c>
+      <c r="F53" s="40">
+        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="H52" s="37"/>
-      <c r="I52" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B8:C8"/>
   </mergeCells>
-  <conditionalFormatting sqref="B10:I52">
-    <cfRule type="expression" dxfId="5" priority="13">
+  <conditionalFormatting sqref="B10:I53">
+    <cfRule type="expression" dxfId="0" priority="13">
       <formula>($C10&gt;=valHStart)*($C10&lt;=valHEnde)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F52">
-    <cfRule type="dataBar" priority="230">
+  <conditionalFormatting sqref="F10:F53">
+    <cfRule type="dataBar" priority="235">
       <dataBar showValue="0">
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2338,7 +2321,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="G6">
       <formula1>lstAufgabenlisteHervorhebungen</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E10:E52">
+    <dataValidation type="list" allowBlank="1" sqref="E10:E53">
       <formula1>"0%,10%,20%,25%,30%,35%,40%,45%,50%,55%,60%,65%,70%,75%,80%,85%,90%,95%,100%"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2359,10 +2342,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F10:F52</xm:sqref>
+          <xm:sqref>F10:F53</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="232" id="{2645DCD5-0397-4C10-8F80-F163C39C9F6D}">
+          <x14:cfRule type="iconSet" priority="237" id="{2645DCD5-0397-4C10-8F80-F163C39C9F6D}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -2378,7 +2361,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>E10:E52</xm:sqref>
+          <xm:sqref>E10:E53</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Inhalt des Commit: Aktualisierung des Zeitplans (vh)
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -277,9 +277,6 @@
     <t>(A) - Animation der Shots 10 - 14</t>
   </si>
   <si>
-    <t>(R) - Rendern des Films + Tonspur + Abspann</t>
-  </si>
-  <si>
     <t>tatsächliche Fertigstellung</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>(S) Kamerafahrt-Szene: Bett +Junge</t>
+  </si>
+  <si>
+    <t>(R) - Zusammenfügen des Films + Tonspur + Abspann</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -626,6 +626,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -636,21 +639,6 @@
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -839,6 +827,21 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4"/>
@@ -918,16 +921,16 @@
     <sortCondition ref="C9:C47"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="11"/>
-    <tableColumn id="7" name="Fällig am" totalsRowDxfId="10"/>
-    <tableColumn id="4" name="Person" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="1" name="% erledigt" totalsRowDxfId="7"/>
-    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="6">
+    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="10"/>
+    <tableColumn id="7" name="Fällig am" totalsRowDxfId="9"/>
+    <tableColumn id="4" name="Person" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="1" name="% erledigt" totalsRowDxfId="6"/>
+    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="5">
       <calculatedColumnFormula>tblAufgabenliste[[#This Row],[% erledigt]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="5"/>
-    <tableColumn id="9" name="tatsächliche Fertigstellung" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="4"/>
+    <tableColumn id="9" name="tatsächliche Fertigstellung" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Project To Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1171,8 +1174,8 @@
   </sheetPr>
   <dimension ref="B1:J53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1267,7 @@
         <v>63</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>62</v>
@@ -1309,7 +1312,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="16">
         <v>1</v>
@@ -1333,7 +1336,7 @@
         <v>39</v>
       </c>
       <c r="E12" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="16">
         <v>1</v>
@@ -1366,7 +1369,9 @@
       <c r="G13" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="15"/>
+      <c r="H13" s="15">
+        <v>42329</v>
+      </c>
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1404,11 +1409,11 @@
         <v>38</v>
       </c>
       <c r="E15" s="16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F15" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>65</v>
@@ -1511,14 +1516,14 @@
         <v>0</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
     <row r="20" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="15">
         <v>42330</v>
@@ -1541,7 +1546,7 @@
     </row>
     <row r="21" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="15">
         <v>42330</v>
@@ -1557,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="41"/>
@@ -1580,7 +1585,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
@@ -1621,13 +1626,17 @@
         <v>38</v>
       </c>
       <c r="E24" s="16">
-        <v>0</v>
-      </c>
-      <c r="F24" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="16">
+        <v>1</v>
+      </c>
       <c r="G24" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="H24" s="13"/>
+        <v>88</v>
+      </c>
+      <c r="H24" s="15">
+        <v>42334</v>
+      </c>
       <c r="I24" s="13"/>
     </row>
     <row r="25" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1641,27 +1650,28 @@
         <v>38</v>
       </c>
       <c r="E25" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="H25" s="13"/>
+        <v>88</v>
+      </c>
+      <c r="H25" s="15">
+        <v>42334</v>
+      </c>
       <c r="I25" s="13"/>
     </row>
     <row r="26" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" s="15">
         <v>42332</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E26" s="16">
         <v>0</v>
@@ -1671,9 +1681,11 @@
         <v>0</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="H26" s="41"/>
+        <v>88</v>
+      </c>
+      <c r="H26" s="45">
+        <v>42334</v>
+      </c>
       <c r="I26" s="41"/>
     </row>
     <row r="27" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1696,7 +1708,9 @@
       <c r="G27" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H27" s="13"/>
+      <c r="H27" s="15">
+        <v>42334</v>
+      </c>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1717,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
@@ -1733,16 +1747,18 @@
         <v>39</v>
       </c>
       <c r="E29" s="16">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="F29" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H29" s="13"/>
+        <v>90</v>
+      </c>
+      <c r="H29" s="15">
+        <v>42331</v>
+      </c>
       <c r="I29" s="13"/>
     </row>
     <row r="30" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1763,7 +1779,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
@@ -1809,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
@@ -1832,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
@@ -1855,7 +1871,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
@@ -1878,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
@@ -1901,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="41"/>
@@ -1924,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H37" s="13"/>
       <c r="I37" s="41"/>
@@ -1947,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H38" s="37"/>
       <c r="I38" s="37"/>
@@ -1970,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
@@ -1993,7 +2009,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
@@ -2039,7 +2055,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
@@ -2062,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
@@ -2085,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="41"/>
@@ -2108,7 +2124,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="41"/>
@@ -2131,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H46" s="37"/>
       <c r="I46" s="37"/>
@@ -2144,7 +2160,7 @@
         <v>42345</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E47" s="16">
         <v>0</v>
@@ -2154,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
@@ -2177,7 +2193,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="41"/>
@@ -2200,7 +2216,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="41"/>
@@ -2223,14 +2239,14 @@
         <v>0</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="13" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C51" s="15">
         <v>42350</v>
@@ -2266,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H52" s="13"/>
       <c r="I52" s="41"/>
@@ -2289,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H53" s="37"/>
       <c r="I53" s="37"/>
@@ -2299,7 +2315,7 @@
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:I53">
-    <cfRule type="expression" dxfId="0" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>($C10&gt;=valHStart)*($C10&lt;=valHEnde)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2445,15 +2461,15 @@
       </c>
       <c r="C7" s="18">
         <f ca="1">TODAY()-WEEKDAY(TODAY(),2)+1</f>
-        <v>42324</v>
+        <v>42331</v>
       </c>
       <c r="D7" s="18">
         <f ca="1">C7+6</f>
-        <v>42330</v>
+        <v>42337</v>
       </c>
       <c r="E7" s="19" t="str">
         <f ca="1">B7&amp;" ["&amp;TEXT(C7,"T MMM")&amp;" - "&amp;TEXT(D7,"T MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Diese Woche [16 Nov - 22 Nov]</v>
+        <v xml:space="preserve">     Diese Woche [23 Nov - 29 Nov]</v>
       </c>
     </row>
     <row r="8" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2524,15 +2540,15 @@
       </c>
       <c r="C12" s="22">
         <f ca="1">C7-7</f>
-        <v>42317</v>
+        <v>42324</v>
       </c>
       <c r="D12" s="22">
         <f ca="1">C12+6</f>
-        <v>42323</v>
+        <v>42330</v>
       </c>
       <c r="E12" s="21" t="str">
         <f ca="1">B12&amp;" ["&amp;TEXT(C12,"T MMM")&amp;" - "&amp;TEXT(D12,"T MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Letzte Woche [9 Nov - 15 Nov]</v>
+        <v xml:space="preserve">     Letzte Woche [16 Nov - 22 Nov]</v>
       </c>
     </row>
     <row r="13" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Inhalt des Commits: aktualisierter Zeitplan (vh)
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -618,6 +618,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -626,9 +629,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1174,8 +1174,8 @@
   </sheetPr>
   <dimension ref="B1:J53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B35" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1238,10 +1238,10 @@
       </c>
     </row>
     <row r="8" spans="2:10" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="43"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1674,16 +1674,15 @@
         <v>42</v>
       </c>
       <c r="E26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H26" s="45">
+      <c r="H26" s="42">
         <v>42334</v>
       </c>
       <c r="I26" s="41"/>
@@ -1699,11 +1698,10 @@
         <v>42</v>
       </c>
       <c r="E27" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>68</v>
@@ -1818,16 +1816,17 @@
         <v>38</v>
       </c>
       <c r="E32" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="H32" s="13"/>
+      <c r="H32" s="15">
+        <v>42335</v>
+      </c>
       <c r="I32" s="13"/>
     </row>
     <row r="33" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1841,16 +1840,18 @@
         <v>39</v>
       </c>
       <c r="E33" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="H33" s="13"/>
+      <c r="H33" s="15">
+        <v>42335</v>
+      </c>
       <c r="I33" s="13"/>
     </row>
     <row r="34" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1864,16 +1865,18 @@
         <v>42</v>
       </c>
       <c r="E34" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="H34" s="13"/>
+      <c r="H34" s="15">
+        <v>42335</v>
+      </c>
       <c r="I34" s="13"/>
     </row>
     <row r="35" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1887,16 +1890,18 @@
         <v>37</v>
       </c>
       <c r="E35" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="H35" s="13"/>
+      <c r="H35" s="15">
+        <v>42335</v>
+      </c>
       <c r="I35" s="13"/>
     </row>
     <row r="36" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2423,12 +2428,12 @@
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
     </row>
     <row r="5" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">

</xml_diff>

<commit_message>
Inhalt des Commits: Aktualisierung des Zeitplans. (vh)
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -1174,8 +1174,8 @@
   </sheetPr>
   <dimension ref="B1:J53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1509,16 +1509,17 @@
         <v>42</v>
       </c>
       <c r="E19" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="15">
+        <v>42337</v>
+      </c>
       <c r="I19" s="13"/>
     </row>
     <row r="20" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1722,16 +1723,18 @@
         <v>75</v>
       </c>
       <c r="E28" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="13"/>
+      <c r="H28" s="15">
+        <v>42337</v>
+      </c>
       <c r="I28" s="13"/>
     </row>
     <row r="29" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1793,16 +1796,17 @@
         <v>42</v>
       </c>
       <c r="E31" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H31" s="13"/>
+      <c r="H31" s="15">
+        <v>42337</v>
+      </c>
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1961,11 +1965,11 @@
         <v>39</v>
       </c>
       <c r="E38" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="40">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="37" t="s">
         <v>86</v>
@@ -2264,7 +2268,7 @@
       </c>
       <c r="F51" s="16"/>
       <c r="G51" s="13" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
@@ -2466,15 +2470,15 @@
       </c>
       <c r="C7" s="18">
         <f ca="1">TODAY()-WEEKDAY(TODAY(),2)+1</f>
-        <v>42331</v>
+        <v>42338</v>
       </c>
       <c r="D7" s="18">
         <f ca="1">C7+6</f>
-        <v>42337</v>
+        <v>42344</v>
       </c>
       <c r="E7" s="19" t="str">
         <f ca="1">B7&amp;" ["&amp;TEXT(C7,"T MMM")&amp;" - "&amp;TEXT(D7,"T MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Diese Woche [23 Nov - 29 Nov]</v>
+        <v xml:space="preserve">     Diese Woche [30 Nov - 6 Dez]</v>
       </c>
     </row>
     <row r="8" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2483,15 +2487,15 @@
       </c>
       <c r="C8" s="22">
         <f ca="1">EOMONTH(TODAY(),-1)+1</f>
-        <v>42309</v>
+        <v>42339</v>
       </c>
       <c r="D8" s="22">
         <f ca="1">EDATE(C8,1)-1</f>
-        <v>42338</v>
+        <v>42369</v>
       </c>
       <c r="E8" s="21" t="str">
         <f ca="1">B8&amp;" ["&amp;TEXT(C8,"T")&amp;" - "&amp;TEXT(D8,"T, MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Dieser Monat [1 - 30, Nov]</v>
+        <v xml:space="preserve">     Dieser Monat [1 - 31, Dez]</v>
       </c>
     </row>
     <row r="9" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2500,15 +2504,15 @@
       </c>
       <c r="C9" s="18">
         <f ca="1">DATE(YEAR(TODAY()),INT(MONTH(TODAY())/3)+1,1)</f>
-        <v>42095</v>
+        <v>42125</v>
       </c>
       <c r="D9" s="18">
         <f ca="1">EDATE(C9,4)-1</f>
-        <v>42216</v>
+        <v>42247</v>
       </c>
       <c r="E9" s="19" t="str">
         <f ca="1">B9&amp;" ["&amp;TEXT(C9,"T MMM")&amp;" - "&amp;TEXT(D9,"T MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Dieses Quartal [1 Apr - 31 Jul]</v>
+        <v xml:space="preserve">     Dieses Quartal [1 Mai - 31 Aug]</v>
       </c>
     </row>
     <row r="10" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2545,15 +2549,15 @@
       </c>
       <c r="C12" s="22">
         <f ca="1">C7-7</f>
-        <v>42324</v>
+        <v>42331</v>
       </c>
       <c r="D12" s="22">
         <f ca="1">C12+6</f>
-        <v>42330</v>
+        <v>42337</v>
       </c>
       <c r="E12" s="21" t="str">
         <f ca="1">B12&amp;" ["&amp;TEXT(C12,"T MMM")&amp;" - "&amp;TEXT(D12,"T MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Letzte Woche [16 Nov - 22 Nov]</v>
+        <v xml:space="preserve">     Letzte Woche [23 Nov - 29 Nov]</v>
       </c>
     </row>
     <row r="13" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2562,15 +2566,15 @@
       </c>
       <c r="C13" s="18">
         <f ca="1">EDATE(C8,-1)</f>
-        <v>42278</v>
+        <v>42309</v>
       </c>
       <c r="D13" s="18">
         <f ca="1">EDATE(C13,1)-1</f>
-        <v>42308</v>
+        <v>42338</v>
       </c>
       <c r="E13" s="19" t="str">
         <f ca="1">B13&amp;" ["&amp;TEXT(C13,"T")&amp;" - "&amp;TEXT(D13,"T, MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Letzter Monat [1 - 31, Okt]</v>
+        <v xml:space="preserve">     Letzter Monat [1 - 30, Nov]</v>
       </c>
     </row>
     <row r="14" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2579,15 +2583,15 @@
       </c>
       <c r="C14" s="22">
         <f ca="1">EDATE(C9,-3)</f>
-        <v>42005</v>
+        <v>42036</v>
       </c>
       <c r="D14" s="22">
         <f ca="1">EDATE(C14,3)-1</f>
-        <v>42094</v>
+        <v>42124</v>
       </c>
       <c r="E14" s="21" t="str">
         <f ca="1">B14&amp;" ["&amp;TEXT(C14,"T MMM")&amp;" - "&amp;TEXT(D14,"T MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Letztes Quartal [1 Jan - 31 Mrz]</v>
+        <v xml:space="preserve">     Letztes Quartal [1 Feb - 30 Apr]</v>
       </c>
     </row>
     <row r="15" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Inhalt des Commit: Anpassung des Zeitplans (vh)
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -307,9 +307,6 @@
     <t>2,5 h</t>
   </si>
   <si>
-    <t xml:space="preserve">4h </t>
-  </si>
-  <si>
     <t>4 h</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>(R) - Zusammenfügen des Films + Tonspur + Abspann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2h </t>
   </si>
 </sst>
 </file>
@@ -1174,8 +1174,8 @@
   </sheetPr>
   <dimension ref="B1:J53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1533,11 +1533,11 @@
         <v>38</v>
       </c>
       <c r="E20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>67</v>
@@ -1556,16 +1556,17 @@
         <v>38</v>
       </c>
       <c r="E21" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H21" s="13"/>
+      <c r="H21" s="15">
+        <v>42341</v>
+      </c>
       <c r="I21" s="41"/>
     </row>
     <row r="22" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1579,11 +1580,11 @@
         <v>39</v>
       </c>
       <c r="E22" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>87</v>
@@ -1666,7 +1667,7 @@
     </row>
     <row r="26" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="15">
         <v>42332</v>
@@ -1916,7 +1917,7 @@
         <v>42336</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E36" s="16">
         <v>0</v>
@@ -1926,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="41"/>
@@ -1939,7 +1940,7 @@
         <v>42336</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E37" s="16">
         <v>0</v>
@@ -1949,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="H37" s="13"/>
       <c r="I37" s="41"/>
@@ -1995,7 +1996,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
@@ -2018,7 +2019,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
@@ -2064,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
@@ -2087,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
@@ -2110,7 +2111,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="41"/>
@@ -2133,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="41"/>
@@ -2179,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
@@ -2202,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="41"/>
@@ -2225,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="41"/>
@@ -2248,14 +2249,14 @@
         <v>0</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C51" s="15">
         <v>42350</v>
@@ -2268,7 +2269,7 @@
       </c>
       <c r="F51" s="16"/>
       <c r="G51" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
@@ -2291,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H52" s="13"/>
       <c r="I52" s="41"/>
@@ -2314,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H53" s="37"/>
       <c r="I53" s="37"/>

</xml_diff>

<commit_message>
animation shot 5-9 auto ueberarbeitet
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktoria Horn\Documents\Studium\3. Semester\03Modul_Medienproduktion\3D-Modellierung und Animation\Projektphase\Nachts-im-Kinderzimmer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janak_000\Documents\HS Fulda\Semester 3\3DMA\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -636,21 +636,6 @@
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -839,6 +824,21 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4"/>
@@ -918,16 +918,16 @@
     <sortCondition ref="C9:C47"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="11"/>
-    <tableColumn id="7" name="Fällig am" totalsRowDxfId="10"/>
-    <tableColumn id="4" name="Person" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="1" name="% erledigt" totalsRowDxfId="7"/>
-    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="6">
+    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="10"/>
+    <tableColumn id="7" name="Fällig am" totalsRowDxfId="9"/>
+    <tableColumn id="4" name="Person" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="1" name="% erledigt" totalsRowDxfId="6"/>
+    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="5">
       <calculatedColumnFormula>tblAufgabenliste[[#This Row],[% erledigt]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="5"/>
-    <tableColumn id="9" name="tatsächliche Fertigstellung" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="4"/>
+    <tableColumn id="9" name="tatsächliche Fertigstellung" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Project To Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1171,29 +1171,29 @@
   </sheetPr>
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.90625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6328125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="21.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1204,12 +1204,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="2:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:10" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="29" t="s">
         <v>26</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:10" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="43" t="s">
         <v>28</v>
       </c>
@@ -1244,7 +1244,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
         <v>41</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
         <v>43</v>
       </c>
@@ -1298,7 +1298,7 @@
       </c>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="13" t="s">
         <v>34</v>
       </c>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13" t="s">
         <v>44</v>
       </c>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
         <v>46</v>
       </c>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="I13" s="15"/>
     </row>
-    <row r="14" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="13" t="s">
         <v>35</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>36</v>
       </c>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="13" t="s">
         <v>59</v>
       </c>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="13" t="s">
         <v>68</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="13" t="s">
         <v>69</v>
       </c>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="13" t="s">
         <v>50</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>82</v>
       </c>
@@ -1542,7 +1542,7 @@
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="13" t="s">
         <v>83</v>
       </c>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="I21" s="41"/>
     </row>
-    <row r="22" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="13" t="s">
         <v>51</v>
       </c>
@@ -1589,7 +1589,7 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="37" t="s">
         <v>30</v>
       </c>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="I23" s="37"/>
     </row>
-    <row r="24" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13" t="s">
         <v>70</v>
       </c>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="13" t="s">
         <v>72</v>
       </c>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
         <v>96</v>
       </c>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="I26" s="41"/>
     </row>
-    <row r="27" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
         <v>71</v>
       </c>
@@ -1710,7 +1710,7 @@
       </c>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="13" t="s">
         <v>47</v>
       </c>
@@ -1735,7 +1735,7 @@
       </c>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>48</v>
       </c>
@@ -1746,11 +1746,11 @@
         <v>39</v>
       </c>
       <c r="E29" s="16">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F29" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>88</v>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="13" t="s">
         <v>67</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="13" t="s">
         <v>49</v>
       </c>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="13" t="s">
         <v>56</v>
       </c>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="13" t="s">
         <v>57</v>
       </c>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="13" t="s">
         <v>58</v>
       </c>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="13" t="s">
         <v>45</v>
       </c>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="13" t="s">
         <v>74</v>
       </c>
@@ -1929,7 +1929,7 @@
       <c r="H36" s="13"/>
       <c r="I36" s="41"/>
     </row>
-    <row r="37" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="13" t="s">
         <v>75</v>
       </c>
@@ -1952,7 +1952,7 @@
       <c r="H37" s="13"/>
       <c r="I37" s="41"/>
     </row>
-    <row r="38" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="37" t="s">
         <v>31</v>
       </c>
@@ -1975,7 +1975,7 @@
       <c r="H38" s="37"/>
       <c r="I38" s="37"/>
     </row>
-    <row r="39" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="13" t="s">
         <v>52</v>
       </c>
@@ -1998,7 +1998,7 @@
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="13" t="s">
         <v>99</v>
       </c>
@@ -2021,7 +2021,7 @@
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="13" t="s">
         <v>53</v>
       </c>
@@ -2044,7 +2044,7 @@
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="13" t="s">
         <v>76</v>
       </c>
@@ -2067,7 +2067,7 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="13" t="s">
         <v>78</v>
       </c>
@@ -2078,11 +2078,11 @@
         <v>39</v>
       </c>
       <c r="E43" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>92</v>
@@ -2090,7 +2090,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="41"/>
     </row>
-    <row r="44" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="13" t="s">
         <v>79</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="H44" s="13"/>
       <c r="I44" s="41"/>
     </row>
-    <row r="45" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="37" t="s">
         <v>32</v>
       </c>
@@ -2136,7 +2136,7 @@
       <c r="H45" s="37"/>
       <c r="I45" s="37"/>
     </row>
-    <row r="46" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="13" t="s">
         <v>54</v>
       </c>
@@ -2159,7 +2159,7 @@
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="13" t="s">
         <v>55</v>
       </c>
@@ -2182,7 +2182,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="41"/>
     </row>
-    <row r="48" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="13" t="s">
         <v>55</v>
       </c>
@@ -2205,7 +2205,7 @@
       <c r="H48" s="13"/>
       <c r="I48" s="41"/>
     </row>
-    <row r="49" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="13" t="s">
         <v>55</v>
       </c>
@@ -2228,7 +2228,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="13" t="s">
         <v>97</v>
       </c>
@@ -2248,7 +2248,7 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="13" t="s">
         <v>77</v>
       </c>
@@ -2271,7 +2271,7 @@
       <c r="H51" s="13"/>
       <c r="I51" s="41"/>
     </row>
-    <row r="52" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="37" t="s">
         <v>33</v>
       </c>
@@ -2299,7 +2299,7 @@
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:I52">
-    <cfRule type="expression" dxfId="0" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>($C10&gt;=valHStart)*($C10&lt;=valHEnde)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2379,17 +2379,17 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="4" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="40" style="4" customWidth="1"/>
-    <col min="4" max="4" width="32.26953125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="36.26953125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="4"/>
+    <col min="4" max="4" width="32.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="1" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" s="1" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2398,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
@@ -2406,7 +2406,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="45" t="s">
         <v>7</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="D4" s="45"/>
       <c r="E4" s="45"/>
     </row>
-    <row r="5" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
         <v>8</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>Keine Hervorhebung</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="30" t="s">
         <v>9</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>15</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v xml:space="preserve">     Diese Woche [30 Nov - 6 Dez]</v>
       </c>
     </row>
-    <row r="8" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="s">
         <v>16</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v xml:space="preserve">     Dieser Monat [1 - 31, Dez]</v>
       </c>
     </row>
-    <row r="9" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>17</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v xml:space="preserve">     Dieses Quartal [1 Mai - 31 Aug]</v>
       </c>
     </row>
-    <row r="10" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
         <v>18</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v xml:space="preserve">     Dieses Jahr [2015]</v>
       </c>
     </row>
-    <row r="11" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="34" t="s">
         <v>9</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>Intervall:</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="s">
         <v>19</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v xml:space="preserve">     Letzte Woche [23 Nov - 29 Nov]</v>
       </c>
     </row>
-    <row r="13" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>20</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v xml:space="preserve">     Letzter Monat [1 - 30, Nov]</v>
       </c>
     </row>
-    <row r="14" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
         <v>21</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v xml:space="preserve">     Letztes Quartal [1 Feb - 30 Apr]</v>
       </c>
     </row>
-    <row r="15" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
         <v>22</v>
       </c>
@@ -2586,13 +2586,13 @@
         <v xml:space="preserve">     Letztes Jahr</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="20"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="21"/>
     </row>
-    <row r="17" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="35" t="s">
         <v>12</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="20" t="s">
         <v>13</v>
       </c>
@@ -2620,7 +2620,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
     </row>
-    <row r="19" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
         <v>14</v>
       </c>
@@ -2631,7 +2631,7 @@
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>

</xml_diff>

<commit_message>
Inhalt des Commits. Aktualisierung des Zeitplans (vh)
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -130,9 +130,6 @@
     <t>Abgabe Beleuchtungsbeispiele</t>
   </si>
   <si>
-    <t>Abgabe finales Video</t>
-  </si>
-  <si>
     <t>Storyboard-Zeichungen</t>
   </si>
   <si>
@@ -259,18 +256,9 @@
     <t>(S) - Bett + Kommode + Junge Szene fertig stellen</t>
   </si>
   <si>
-    <t>(A) - Animation der Shots 1-4</t>
-  </si>
-  <si>
     <t>(P) - evtl. Postproduction</t>
   </si>
   <si>
-    <t xml:space="preserve">(A) - Animation der Shots 5 - 9 </t>
-  </si>
-  <si>
-    <t>(A) - Animation der Shots 10 - 14</t>
-  </si>
-  <si>
     <t>tatsächliche Fertigstellung</t>
   </si>
   <si>
@@ -329,6 +317,18 @@
   </si>
   <si>
     <t>Beleuchtung - Morgensonne</t>
+  </si>
+  <si>
+    <t>(A) - Animation der Shots 6 - 10</t>
+  </si>
+  <si>
+    <t>(A) - Animation der Shots 1-5 + 13</t>
+  </si>
+  <si>
+    <t>(A) - Animation der Shots 11 - 15, außer 13</t>
+  </si>
+  <si>
+    <t>Abgabe finales Video + Präsentation</t>
   </si>
 </sst>
 </file>
@@ -636,21 +636,6 @@
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -839,6 +824,21 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4"/>
@@ -918,16 +918,16 @@
     <sortCondition ref="C9:C47"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="11"/>
-    <tableColumn id="7" name="Fällig am" totalsRowDxfId="10"/>
-    <tableColumn id="4" name="Person" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="1" name="% erledigt" totalsRowDxfId="7"/>
-    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="6">
+    <tableColumn id="2" name="Aufgaben" totalsRowDxfId="10"/>
+    <tableColumn id="7" name="Fällig am" totalsRowDxfId="9"/>
+    <tableColumn id="4" name="Person" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="1" name="% erledigt" totalsRowDxfId="6"/>
+    <tableColumn id="6" name="Fortschritt" totalsRowDxfId="5">
       <calculatedColumnFormula>tblAufgabenliste[[#This Row],[% erledigt]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="5"/>
-    <tableColumn id="9" name="tatsächliche Fertigstellung" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="Zeitaufwand (h)" totalsRowDxfId="4"/>
+    <tableColumn id="9" name="tatsächliche Fertigstellung" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="3" name="Risiken + Lösungen" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Project To Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1171,8 +1171,8 @@
   </sheetPr>
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="9" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>3</v>
@@ -1261,13 +1261,13 @@
         <v>5</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>1</v>
@@ -1275,13 +1275,13 @@
     </row>
     <row r="10" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="15">
         <v>42324</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="16">
         <v>1</v>
@@ -1291,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="15">
         <v>42324</v>
@@ -1300,13 +1300,13 @@
     </row>
     <row r="11" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="15">
         <v>42326</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="16">
         <v>1</v>
@@ -1315,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H11" s="15">
         <v>42324</v>
@@ -1324,13 +1324,13 @@
     </row>
     <row r="12" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="15">
         <v>42326</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="16">
         <v>1</v>
@@ -1339,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H12" s="15">
         <v>42328</v>
@@ -1348,13 +1348,13 @@
     </row>
     <row r="13" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="15">
         <v>42328</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13" s="16">
         <v>1</v>
@@ -1364,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" s="15">
         <v>42329</v>
@@ -1373,13 +1373,13 @@
     </row>
     <row r="14" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="15">
         <v>42328</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="16">
         <v>1</v>
@@ -1388,7 +1388,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H14" s="15">
         <v>42328</v>
@@ -1397,13 +1397,13 @@
     </row>
     <row r="15" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="15">
         <v>42328</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="16">
         <v>1</v>
@@ -1413,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H15" s="15">
         <v>42329</v>
@@ -1422,13 +1422,13 @@
     </row>
     <row r="16" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="15">
         <v>42329</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="16">
         <v>1</v>
@@ -1438,7 +1438,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="15">
         <v>42327</v>
@@ -1447,13 +1447,13 @@
     </row>
     <row r="17" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="15">
         <v>42329</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="16">
         <v>1</v>
@@ -1463,7 +1463,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" s="15">
         <v>42328</v>
@@ -1472,13 +1472,13 @@
     </row>
     <row r="18" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="15">
         <v>42329</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="16">
         <v>1</v>
@@ -1488,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18" s="15">
         <v>42327</v>
@@ -1497,13 +1497,13 @@
     </row>
     <row r="19" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="15">
         <v>42330</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="16">
         <v>1</v>
@@ -1512,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H19" s="15">
         <v>42337</v>
@@ -1521,13 +1521,13 @@
     </row>
     <row r="20" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C20" s="15">
         <v>42330</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E20" s="16">
         <v>1</v>
@@ -1537,20 +1537,22 @@
         <v>1</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="13"/>
+        <v>64</v>
+      </c>
+      <c r="H20" s="15">
+        <v>42342</v>
+      </c>
       <c r="I20" s="13"/>
     </row>
     <row r="21" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C21" s="15">
         <v>42330</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="16">
         <v>1</v>
@@ -1559,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H21" s="15">
         <v>42341</v>
@@ -1568,13 +1570,13 @@
     </row>
     <row r="22" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="15">
         <v>42330</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="16">
         <v>1</v>
@@ -1584,9 +1586,11 @@
         <v>1</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="H22" s="13"/>
+        <v>81</v>
+      </c>
+      <c r="H22" s="15">
+        <v>42341</v>
+      </c>
       <c r="I22" s="13"/>
     </row>
     <row r="23" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1597,7 +1601,7 @@
         <v>42330</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" s="40">
         <v>1</v>
@@ -1607,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H23" s="38">
         <v>42329</v>
@@ -1616,13 +1620,13 @@
     </row>
     <row r="24" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="15">
         <v>42332</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" s="16">
         <v>1</v>
@@ -1631,7 +1635,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H24" s="15">
         <v>42334</v>
@@ -1640,13 +1644,13 @@
     </row>
     <row r="25" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" s="15">
         <v>42332</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="16">
         <v>1</v>
@@ -1655,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H25" s="15">
         <v>42334</v>
@@ -1664,13 +1668,13 @@
     </row>
     <row r="26" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C26" s="15">
         <v>42332</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E26" s="16">
         <v>1</v>
@@ -1679,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H26" s="42">
         <v>42334</v>
@@ -1688,13 +1692,13 @@
     </row>
     <row r="27" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="15">
         <v>42332</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" s="16">
         <v>1</v>
@@ -1703,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H27" s="15">
         <v>42334</v>
@@ -1712,13 +1716,13 @@
     </row>
     <row r="28" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="15">
         <v>42333</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" s="16">
         <v>1</v>
@@ -1728,7 +1732,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H28" s="15">
         <v>42337</v>
@@ -1737,23 +1741,23 @@
     </row>
     <row r="29" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="15">
         <v>42333</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E29" s="16">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F29" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H29" s="15">
         <v>42331</v>
@@ -1762,36 +1766,38 @@
     </row>
     <row r="30" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" s="15">
         <v>42333</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E30" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="H30" s="13"/>
+        <v>84</v>
+      </c>
+      <c r="H30" s="15">
+        <v>42342</v>
+      </c>
       <c r="I30" s="13"/>
     </row>
     <row r="31" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="15">
         <v>42333</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E31" s="16">
         <v>1</v>
@@ -1800,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H31" s="15">
         <v>42337</v>
@@ -1809,13 +1815,13 @@
     </row>
     <row r="32" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="15">
         <v>42334</v>
       </c>
       <c r="D32" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32" s="16">
         <v>1</v>
@@ -1824,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H32" s="15">
         <v>42335</v>
@@ -1833,13 +1839,13 @@
     </row>
     <row r="33" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="15">
         <v>42334</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E33" s="16">
         <v>1</v>
@@ -1849,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H33" s="15">
         <v>42335</v>
@@ -1858,13 +1864,13 @@
     </row>
     <row r="34" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="15">
         <v>42334</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E34" s="16">
         <v>1</v>
@@ -1874,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H34" s="15">
         <v>42335</v>
@@ -1883,13 +1889,13 @@
     </row>
     <row r="35" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="15">
         <v>42335</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E35" s="16">
         <v>1</v>
@@ -1899,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H35" s="15">
         <v>42335</v>
@@ -1908,48 +1914,51 @@
     </row>
     <row r="36" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="15">
         <v>42336</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E36" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H36" s="13"/>
+        <v>65</v>
+      </c>
+      <c r="H36" s="15">
+        <v>42343</v>
+      </c>
       <c r="I36" s="41"/>
     </row>
     <row r="37" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="15">
         <v>42336</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="H37" s="13"/>
+        <v>94</v>
+      </c>
+      <c r="H37" s="15">
+        <v>42343</v>
+      </c>
       <c r="I37" s="41"/>
     </row>
     <row r="38" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1960,7 +1969,7 @@
         <v>42337</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E38" s="40">
         <v>1</v>
@@ -1970,20 +1979,20 @@
         <v>1</v>
       </c>
       <c r="G38" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H38" s="37"/>
       <c r="I38" s="37"/>
     </row>
     <row r="39" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="15">
         <v>42340</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E39" s="16">
         <v>0</v>
@@ -1993,43 +2002,44 @@
         <v>0</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H39" s="13"/>
+        <v>87</v>
+      </c>
+      <c r="H39" s="15">
+        <v>42343</v>
+      </c>
       <c r="I39" s="13"/>
     </row>
     <row r="40" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C40" s="15">
         <v>42340</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E40" s="16">
-        <v>0</v>
-      </c>
-      <c r="F40" s="16">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F40" s="16"/>
       <c r="G40" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H40" s="13"/>
+        <v>61</v>
+      </c>
+      <c r="H40" s="15">
+        <v>42343</v>
+      </c>
       <c r="I40" s="13"/>
     </row>
     <row r="41" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" s="15">
         <v>42341</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E41" s="16">
         <v>0</v>
@@ -2039,20 +2049,22 @@
         <v>0</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H41" s="13"/>
+        <v>87</v>
+      </c>
+      <c r="H41" s="15">
+        <v>42343</v>
+      </c>
       <c r="I41" s="13"/>
     </row>
     <row r="42" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="13" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="C42" s="15">
         <v>42343</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E42" s="16">
         <v>0</v>
@@ -2062,20 +2074,20 @@
         <v>0</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
     <row r="43" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="13" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C43" s="15">
         <v>42343</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E43" s="16">
         <v>0</v>
@@ -2085,20 +2097,20 @@
         <v>0</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="41"/>
     </row>
     <row r="44" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="13" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C44" s="15">
         <v>42343</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E44" s="16">
         <v>0</v>
@@ -2108,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="41"/>
@@ -2121,7 +2133,7 @@
         <v>42344</v>
       </c>
       <c r="D45" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E45" s="40">
         <v>0</v>
@@ -2131,20 +2143,20 @@
         <v>0</v>
       </c>
       <c r="G45" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H45" s="37"/>
       <c r="I45" s="37"/>
     </row>
     <row r="46" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46" s="15">
-        <v>42345</v>
+        <v>42350</v>
       </c>
       <c r="D46" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E46" s="16">
         <v>0</v>
@@ -2154,20 +2166,20 @@
         <v>0</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
     </row>
     <row r="47" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C47" s="15">
         <v>42347</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E47" s="16">
         <v>0</v>
@@ -2177,20 +2189,20 @@
         <v>0</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="41"/>
     </row>
     <row r="48" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="15">
         <v>42348</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E48" s="16">
         <v>0</v>
@@ -2200,20 +2212,20 @@
         <v>0</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="41"/>
     </row>
     <row r="49" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="15">
         <v>42349</v>
       </c>
       <c r="D49" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E49" s="16">
         <v>0</v>
@@ -2223,40 +2235,40 @@
         <v>0</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C50" s="15">
         <v>42350</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E50" s="16">
         <v>0</v>
       </c>
       <c r="F50" s="16"/>
       <c r="G50" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C51" s="15">
         <v>42350</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E51" s="16">
         <v>0</v>
@@ -2266,20 +2278,20 @@
         <v>0</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H51" s="13"/>
       <c r="I51" s="41"/>
     </row>
     <row r="52" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="37" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C52" s="38">
         <v>42351</v>
       </c>
       <c r="D52" s="39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E52" s="40">
         <v>0</v>
@@ -2289,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="37" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H52" s="37"/>
       <c r="I52" s="37"/>
@@ -2299,7 +2311,7 @@
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:I52">
-    <cfRule type="expression" dxfId="0" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>($C10&gt;=valHStart)*($C10&lt;=valHEnde)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Inhalt des Commits: Aktualisierung des Zeitplans für die finale Präsentation (vh)
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="101">
   <si>
     <t>Start:</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>Abgabe finales Video + Präsentation</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1175,7 @@
   <dimension ref="B1:J52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1995,11 +1998,11 @@
         <v>41</v>
       </c>
       <c r="E39" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>87</v>
@@ -2042,11 +2045,11 @@
         <v>36</v>
       </c>
       <c r="E41" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>87</v>
@@ -2067,16 +2070,18 @@
         <v>37</v>
       </c>
       <c r="E42" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H42" s="13"/>
+      <c r="H42" s="15">
+        <v>42345</v>
+      </c>
       <c r="I42" s="13"/>
     </row>
     <row r="43" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2090,16 +2095,18 @@
         <v>38</v>
       </c>
       <c r="E43" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H43" s="13"/>
+      <c r="H43" s="15">
+        <v>42345</v>
+      </c>
       <c r="I43" s="41"/>
     </row>
     <row r="44" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2113,16 +2120,18 @@
         <v>41</v>
       </c>
       <c r="E44" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H44" s="13"/>
+      <c r="H44" s="15">
+        <v>42345</v>
+      </c>
       <c r="I44" s="41"/>
     </row>
     <row r="45" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2136,16 +2145,18 @@
         <v>41</v>
       </c>
       <c r="E45" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="40">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="H45" s="37"/>
+      <c r="H45" s="38">
+        <v>42344</v>
+      </c>
       <c r="I45" s="37"/>
     </row>
     <row r="46" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2159,16 +2170,18 @@
         <v>39</v>
       </c>
       <c r="E46" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="H46" s="13"/>
+      <c r="H46" s="15">
+        <v>42346</v>
+      </c>
       <c r="I46" s="13"/>
     </row>
     <row r="47" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2182,16 +2195,18 @@
         <v>36</v>
       </c>
       <c r="E47" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="H47" s="13"/>
+      <c r="H47" s="15">
+        <v>42345</v>
+      </c>
       <c r="I47" s="41"/>
     </row>
     <row r="48" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2205,16 +2220,18 @@
         <v>36</v>
       </c>
       <c r="E48" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="H48" s="13"/>
+      <c r="H48" s="15">
+        <v>42346</v>
+      </c>
       <c r="I48" s="41"/>
     </row>
     <row r="49" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2228,16 +2245,18 @@
         <v>36</v>
       </c>
       <c r="E49" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="H49" s="13"/>
+      <c r="H49" s="15">
+        <v>42347</v>
+      </c>
       <c r="I49" s="13"/>
     </row>
     <row r="50" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2293,12 +2312,12 @@
       <c r="D52" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="40">
-        <v>0</v>
-      </c>
-      <c r="F52" s="40">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+      <c r="E52" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="F52" s="40" t="str">
+        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
+        <v>%</v>
       </c>
       <c r="G52" s="37" t="s">
         <v>91</v>
@@ -2457,15 +2476,15 @@
       </c>
       <c r="C7" s="18">
         <f ca="1">TODAY()-WEEKDAY(TODAY(),2)+1</f>
-        <v>42338</v>
+        <v>42345</v>
       </c>
       <c r="D7" s="18">
         <f ca="1">C7+6</f>
-        <v>42344</v>
+        <v>42351</v>
       </c>
       <c r="E7" s="19" t="str">
         <f ca="1">B7&amp;" ["&amp;TEXT(C7,"T MMM")&amp;" - "&amp;TEXT(D7,"T MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Diese Woche [30 Nov - 6 Dez]</v>
+        <v xml:space="preserve">     Diese Woche [7 Dez - 13 Dez]</v>
       </c>
     </row>
     <row r="8" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2536,15 +2555,15 @@
       </c>
       <c r="C12" s="22">
         <f ca="1">C7-7</f>
-        <v>42331</v>
+        <v>42338</v>
       </c>
       <c r="D12" s="22">
         <f ca="1">C12+6</f>
-        <v>42337</v>
+        <v>42344</v>
       </c>
       <c r="E12" s="21" t="str">
         <f ca="1">B12&amp;" ["&amp;TEXT(C12,"T MMM")&amp;" - "&amp;TEXT(D12,"T MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Letzte Woche [23 Nov - 29 Nov]</v>
+        <v xml:space="preserve">     Letzte Woche [30 Nov - 6 Dez]</v>
       </c>
     </row>
     <row r="13" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Inhalt des Commits: Wahrscheinlich letzte Akrualisierung des Zeitplans (vh)
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="102">
   <si>
     <t>Start:</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -1174,8 +1177,8 @@
   </sheetPr>
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1984,7 +1987,9 @@
       <c r="G38" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="H38" s="37"/>
+      <c r="H38" s="38">
+        <v>42336</v>
+      </c>
       <c r="I38" s="37"/>
     </row>
     <row r="39" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2025,7 +2030,9 @@
       <c r="E40" s="16">
         <v>1</v>
       </c>
-      <c r="F40" s="16"/>
+      <c r="F40" s="16">
+        <v>1</v>
+      </c>
       <c r="G40" s="13" t="s">
         <v>61</v>
       </c>
@@ -2270,13 +2277,17 @@
         <v>36</v>
       </c>
       <c r="E50" s="16">
-        <v>0</v>
-      </c>
-      <c r="F50" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F50" s="16">
+        <v>1</v>
+      </c>
       <c r="G50" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H50" s="13"/>
+      <c r="H50" s="15">
+        <v>42350</v>
+      </c>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2289,9 +2300,7 @@
       <c r="D51" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="16">
-        <v>0</v>
-      </c>
+      <c r="E51" s="16"/>
       <c r="F51" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
         <v>0</v>
@@ -2299,7 +2308,9 @@
       <c r="G51" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H51" s="13"/>
+      <c r="H51" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="I51" s="41"/>
     </row>
     <row r="52" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2322,7 +2333,9 @@
       <c r="G52" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="H52" s="37"/>
+      <c r="H52" s="38">
+        <v>42351</v>
+      </c>
       <c r="I52" s="37"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inhalt des Commits: Letzte Aktualisierung des Zeitplans. Es ist geschafft! (vh)
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="101">
   <si>
     <t>Start:</t>
   </si>
@@ -329,9 +329,6 @@
   </si>
   <si>
     <t>Abgabe finales Video + Präsentation</t>
-  </si>
-  <si>
-    <t>%</t>
   </si>
   <si>
     <t>/</t>
@@ -1177,8 +1174,8 @@
   </sheetPr>
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1187,10 +1184,10 @@
     <col min="2" max="2" width="46.6328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.90625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.81640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
@@ -2309,7 +2306,7 @@
         <v>86</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I51" s="41"/>
     </row>
@@ -2323,12 +2320,12 @@
       <c r="D52" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="F52" s="40" t="str">
-        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>%</v>
+      <c r="E52" s="40">
+        <v>1</v>
+      </c>
+      <c r="F52" s="40">
+        <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
+        <v>1</v>
       </c>
       <c r="G52" s="37" t="s">
         <v>91</v>

</xml_diff>